<commit_message>
add logic to create testNg file into project
</commit_message>
<xml_diff>
--- a/test-output/excel-report.xlsx
+++ b/test-output/excel-report.xlsx
@@ -284,14 +284,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true" showGridLines="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="13.890625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="27.84765625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.57421875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="23.20703125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -367,18 +367,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="46.7890625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="10.62109375" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.609375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="27.46484375" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="27.84765625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.0859375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="38.98828125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="8.84765625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="12.17578125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="22.88671875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="23.20703125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.90234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>